<commit_message>
creacion de confirmar colacion
</commit_message>
<xml_diff>
--- a/sistema_de_alimentacion.xlsx
+++ b/sistema_de_alimentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\.Hospital\MinutaHospital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37459D20-B767-44F5-B660-884EE8118B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305777EB-A975-4A33-AC59-D099036BC496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="925" firstSheet="1" activeTab="13" xr2:uid="{8554B5AA-75F9-4A04-86C5-EC624286FE63}"/>
   </bookViews>
@@ -5675,24 +5675,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5716,6 +5701,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5723,6 +5711,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -19790,23 +19790,23 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="101"/>
-      <c r="S3" s="101"/>
-      <c r="T3" s="101"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
@@ -19823,7 +19823,7 @@
       <c r="F5" s="71"/>
     </row>
     <row r="6" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="107" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="85"/>
@@ -19835,7 +19835,7 @@
       <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="107" t="s">
         <v>267</v>
       </c>
       <c r="B8" s="85"/>
@@ -19848,7 +19848,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
       <c r="E9" t="s">
@@ -19867,14 +19867,14 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="107" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="85"/>
       <c r="C11" s="85"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="85"/>
       <c r="C12" s="85"/>
     </row>
@@ -19971,21 +19971,21 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="105" t="s">
         <v>282</v>
       </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="106"/>
       <c r="E24" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="105" t="s">
         <v>283</v>
       </c>
-      <c r="B25" s="97"/>
-      <c r="C25" s="97"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="52"/>
@@ -20077,7 +20077,7 @@
   <dimension ref="A2:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20132,7 +20132,7 @@
       <c r="E3" s="29" t="s">
         <v>1259</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="29" t="s">
         <v>1260</v>
       </c>
       <c r="G3" s="29" t="s">
@@ -20147,7 +20147,7 @@
       <c r="J3" s="29" t="s">
         <v>1266</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="29" t="s">
         <v>1269</v>
       </c>
     </row>
@@ -55920,22 +55920,22 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33"/>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
       <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
       <c r="G5" s="34"/>
       <c r="K5" s="30" t="s">
         <v>17</v>
@@ -55953,15 +55953,15 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
-      <c r="B7" s="92">
+      <c r="B7" s="93">
         <v>1</v>
       </c>
       <c r="C7" s="35"/>
-      <c r="D7" s="92">
+      <c r="D7" s="93">
         <v>2</v>
       </c>
       <c r="E7" s="35"/>
-      <c r="F7" s="92">
+      <c r="F7" s="93">
         <v>3</v>
       </c>
       <c r="G7" s="34"/>
@@ -55972,11 +55972,11 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
-      <c r="B8" s="92"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="35"/>
-      <c r="D8" s="92"/>
+      <c r="D8" s="93"/>
       <c r="E8" s="35"/>
-      <c r="F8" s="92"/>
+      <c r="F8" s="93"/>
       <c r="G8" s="34"/>
       <c r="K8" s="36" t="s">
         <v>321</v>
@@ -55990,26 +55990,26 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
-      <c r="B10" s="92">
+      <c r="B10" s="93">
         <v>4</v>
       </c>
       <c r="C10" s="35"/>
-      <c r="D10" s="92">
+      <c r="D10" s="93">
         <v>5</v>
       </c>
       <c r="E10" s="35"/>
-      <c r="F10" s="92">
+      <c r="F10" s="93">
         <v>6</v>
       </c>
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
-      <c r="B11" s="92"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="35"/>
-      <c r="D11" s="92"/>
+      <c r="D11" s="93"/>
       <c r="E11" s="35"/>
-      <c r="F11" s="92"/>
+      <c r="F11" s="93"/>
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -56018,26 +56018,26 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
-      <c r="B13" s="92">
+      <c r="B13" s="93">
         <v>7</v>
       </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="92">
+      <c r="D13" s="93">
         <v>8</v>
       </c>
       <c r="E13" s="35"/>
-      <c r="F13" s="92">
+      <c r="F13" s="93">
         <v>9</v>
       </c>
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
-      <c r="B14" s="92"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="35"/>
-      <c r="D14" s="92"/>
+      <c r="D14" s="93"/>
       <c r="E14" s="35"/>
-      <c r="F14" s="92"/>
+      <c r="F14" s="93"/>
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -56046,24 +56046,24 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
-      <c r="B16" s="92"/>
+      <c r="B16" s="93"/>
       <c r="C16" s="35"/>
-      <c r="D16" s="92">
+      <c r="D16" s="93">
         <v>0</v>
       </c>
       <c r="E16" s="35"/>
-      <c r="F16" s="92" t="s">
+      <c r="F16" s="93" t="s">
         <v>270</v>
       </c>
       <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
-      <c r="B17" s="92"/>
+      <c r="B17" s="93"/>
       <c r="C17" s="35"/>
-      <c r="D17" s="92"/>
+      <c r="D17" s="93"/>
       <c r="E17" s="35"/>
-      <c r="F17" s="92"/>
+      <c r="F17" s="93"/>
       <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -56072,22 +56072,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="93" t="s">
         <v>269</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
       <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
       <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -56110,12 +56110,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
     <mergeCell ref="B19:F20"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D7:D8"/>
@@ -56124,6 +56118,12 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -58184,47 +58184,47 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="101"/>
-      <c r="S3" s="101"/>
-      <c r="T3" s="101"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="96"/>
+      <c r="S3" s="96"/>
+      <c r="T3" s="96"/>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="102" t="s">
         <v>277</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="107"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="103"/>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
@@ -58246,10 +58246,10 @@
       <c r="Q5" s="87"/>
       <c r="R5" s="87"/>
       <c r="S5" s="87"/>
-      <c r="T5" s="108"/>
+      <c r="T5" s="104"/>
     </row>
     <row r="6" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="107" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="85"/>
@@ -58294,7 +58294,7 @@
       <c r="T7" s="55"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="107" t="s">
         <v>267</v>
       </c>
       <c r="B8" s="85"/>
@@ -58324,7 +58324,7 @@
       <c r="T8" s="55"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="85"/>
       <c r="C9" s="85"/>
       <c r="D9" s="6"/>
@@ -58368,7 +58368,7 @@
       <c r="T10" s="55"/>
     </row>
     <row r="11" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="107" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="85"/>
@@ -58392,7 +58392,7 @@
       <c r="T11" s="55"/>
     </row>
     <row r="12" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="85"/>
       <c r="C12" s="85"/>
       <c r="D12" s="3" t="s">
@@ -58425,10 +58425,10 @@
       <c r="M12" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="95"/>
-      <c r="O12" s="95"/>
-      <c r="P12" s="95"/>
-      <c r="Q12" s="95"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
       <c r="R12" s="47" t="s">
         <v>292</v>
       </c>
@@ -58460,32 +58460,32 @@
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
-      <c r="D14" s="98">
-        <v>2</v>
-      </c>
-      <c r="E14" s="98" t="s">
+      <c r="D14" s="101">
+        <v>2</v>
+      </c>
+      <c r="E14" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="98" t="s">
+      <c r="F14" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="98">
+      <c r="G14" s="101">
         <v>42</v>
       </c>
-      <c r="H14" s="98" t="s">
+      <c r="H14" s="101" t="s">
         <v>289</v>
       </c>
-      <c r="I14" s="98" t="s">
+      <c r="I14" s="101" t="s">
         <v>290</v>
       </c>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="102"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="99"/>
+      <c r="P14" s="99"/>
+      <c r="Q14" s="99"/>
       <c r="S14" s="49"/>
       <c r="T14" s="55"/>
     </row>
@@ -58493,20 +58493,20 @@
       <c r="A15" s="53"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="100"/>
-      <c r="K15" s="100"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="105"/>
-      <c r="O15" s="105"/>
-      <c r="P15" s="105"/>
-      <c r="Q15" s="105"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="100"/>
       <c r="S15" s="49"/>
       <c r="T15" s="55"/>
     </row>
@@ -58602,19 +58602,19 @@
       <c r="T23" s="55"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="105" t="s">
         <v>282</v>
       </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="106"/>
       <c r="T24" s="55"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="105" t="s">
         <v>283</v>
       </c>
-      <c r="B25" s="97"/>
-      <c r="C25" s="97"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
       <c r="T25" s="55"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -58722,6 +58722,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="A11:C12"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="D1:T3"/>
     <mergeCell ref="L14:L15"/>
@@ -58735,17 +58746,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="D4:T5"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="A11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>